<commit_message>
nb: separating pilot 1 and pilot 2
</commit_message>
<xml_diff>
--- a/results/2023_08_08_trial_labeling/channel_mapping.xlsx
+++ b/results/2023_08_08_trial_labeling/channel_mapping.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26803"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="94" documentId="11_0F4F44A19DA2FD9B0909FF3BF4FFFF8AEA66B218" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{20651217-0FF3-4074-A166-3086B63E6C57}"/>
+  <xr:revisionPtr revIDLastSave="109" documentId="11_0F4F44A19DA2FD9B0909FF3BF4FFFF8AEA66B218" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4006EE33-D725-4757-BEDC-BC3362E4F2EF}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -420,8 +420,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -477,7 +477,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1">
-        <v>1.1000000000000001</v>
+        <v>6.1</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1">
@@ -493,17 +493,25 @@
         <v>31</v>
       </c>
       <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
+      <c r="I2" s="1">
+        <v>15</v>
+      </c>
+      <c r="J2" s="1">
+        <v>14</v>
+      </c>
+      <c r="K2" s="1">
+        <v>13</v>
+      </c>
+      <c r="L2" s="1">
+        <v>16</v>
+      </c>
     </row>
     <row r="3" spans="1:12">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" s="1">
-        <v>1.2</v>
+        <v>6.2</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1">
@@ -529,7 +537,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="1">
-        <v>1.3</v>
+        <v>6.3</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1">
@@ -555,7 +563,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="1">
-        <v>1.4</v>
+        <v>6.4</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1">
@@ -668,11 +676,21 @@
       <c r="G8" s="1">
         <v>12</v>
       </c>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
-      <c r="L8" s="1"/>
+      <c r="H8" s="1">
+        <v>9</v>
+      </c>
+      <c r="I8" s="1">
+        <v>31</v>
+      </c>
+      <c r="J8" s="1">
+        <v>30</v>
+      </c>
+      <c r="K8" s="1">
+        <v>29</v>
+      </c>
+      <c r="L8" s="1">
+        <v>28</v>
+      </c>
     </row>
     <row r="9" spans="1:12">
       <c r="A9" s="1">
@@ -695,7 +713,7 @@
         <v>12</v>
       </c>
       <c r="H9" s="1">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="I9" s="1">
         <v>31</v>
@@ -716,26 +734,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="66c7fa70-bb82-47de-8c9f-8b3ecea6303f" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="05f64c5e-7ec2-4cf0-a148-a77e53878df3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002C00C86E44419345A6E3C05C9040286D" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="75e447aa01971d87755e32be9f432ab5">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="05f64c5e-7ec2-4cf0-a148-a77e53878df3" xmlns:ns3="66c7fa70-bb82-47de-8c9f-8b3ecea6303f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="128ff4447dd710e229a73405da0381bf" ns2:_="" ns3:_="">
     <xsd:import namespace="05f64c5e-7ec2-4cf0-a148-a77e53878df3"/>
@@ -978,8 +976,28 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="66c7fa70-bb82-47de-8c9f-8b3ecea6303f" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="05f64c5e-7ec2-4cf0-a148-a77e53878df3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2CAEC680-0A4F-4180-A403-8A817B185CC8}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4B9F624A-309C-4C3F-AD98-5266832A082A}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -987,5 +1005,5 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4B9F624A-309C-4C3F-AD98-5266832A082A}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2CAEC680-0A4F-4180-A403-8A817B185CC8}"/>
 </file>
</xml_diff>

<commit_message>
nb: log scale for lfp power
</commit_message>
<xml_diff>
--- a/results/2023_08_08_trial_labeling/channel_mapping.xlsx
+++ b/results/2023_08_08_trial_labeling/channel_mapping.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26803"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="109" documentId="11_0F4F44A19DA2FD9B0909FF3BF4FFFF8AEA66B218" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4006EE33-D725-4757-BEDC-BC3362E4F2EF}"/>
+  <xr:revisionPtr revIDLastSave="110" documentId="11_0F4F44A19DA2FD9B0909FF3BF4FFFF8AEA66B218" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6DF869E0-0A3B-4C9D-B9B2-6C83268E7ED2}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -421,7 +421,7 @@
   <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -492,7 +492,9 @@
       <c r="G2" s="1">
         <v>31</v>
       </c>
-      <c r="H2" s="1"/>
+      <c r="H2" s="1">
+        <v>21</v>
+      </c>
       <c r="I2" s="1">
         <v>15</v>
       </c>
@@ -734,6 +736,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="66c7fa70-bb82-47de-8c9f-8b3ecea6303f" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="05f64c5e-7ec2-4cf0-a148-a77e53878df3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002C00C86E44419345A6E3C05C9040286D" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="75e447aa01971d87755e32be9f432ab5">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="05f64c5e-7ec2-4cf0-a148-a77e53878df3" xmlns:ns3="66c7fa70-bb82-47de-8c9f-8b3ecea6303f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="128ff4447dd710e229a73405da0381bf" ns2:_="" ns3:_="">
     <xsd:import namespace="05f64c5e-7ec2-4cf0-a148-a77e53878df3"/>
@@ -976,28 +998,8 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="66c7fa70-bb82-47de-8c9f-8b3ecea6303f" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="05f64c5e-7ec2-4cf0-a148-a77e53878df3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4B9F624A-309C-4C3F-AD98-5266832A082A}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2CAEC680-0A4F-4180-A403-8A817B185CC8}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1005,5 +1007,5 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2CAEC680-0A4F-4180-A403-8A817B185CC8}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4B9F624A-309C-4C3F-AD98-5266832A082A}"/>
 </file>
</xml_diff>